<commit_message>
complete register new user test
</commit_message>
<xml_diff>
--- a/UsersForRegisterTestMatadoryValid.xlsx
+++ b/UsersForRegisterTestMatadoryValid.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>email</t>
   </si>
@@ -81,57 +81,24 @@
     <t>community</t>
   </si>
   <si>
-    <t>Lviv</t>
-  </si>
-  <si>
-    <t>СВ</t>
-  </si>
-  <si>
-    <t>Shevchenkivskym</t>
-  </si>
-  <si>
     <t>Ivan</t>
   </si>
   <si>
     <t>Freude</t>
   </si>
   <si>
-    <t>Salti</t>
-  </si>
-  <si>
     <t>salti@email.com</t>
   </si>
   <si>
     <t>salti</t>
   </si>
   <si>
-    <t>Levandivka</t>
-  </si>
-  <si>
-    <t>Zahid</t>
-  </si>
-  <si>
-    <t>Kubiva</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>79000</t>
-  </si>
-  <si>
     <t>Liza</t>
   </si>
   <si>
     <t>Otto</t>
   </si>
   <si>
-    <t>Grygorivna</t>
-  </si>
-  <si>
     <t>otto@email.com</t>
   </si>
   <si>
@@ -144,18 +111,12 @@
     <t>Bekham</t>
   </si>
   <si>
-    <t>Pylypoxych</t>
-  </si>
-  <si>
     <t>Petro</t>
   </si>
   <si>
     <t>Poroshenko</t>
   </si>
   <si>
-    <t>Roshenovych</t>
-  </si>
-  <si>
     <t>cykerochka@email.com</t>
   </si>
   <si>
@@ -168,9 +129,6 @@
     <t>Kozhemyakovych</t>
   </si>
   <si>
-    <t>Mestnyi</t>
-  </si>
-  <si>
     <t>goroshko@email.com</t>
   </si>
   <si>
@@ -189,9 +147,6 @@
     <t>Mandrykovskyy</t>
   </si>
   <si>
-    <t>Mandryk</t>
-  </si>
-  <si>
     <t>mandryk@email.com</t>
   </si>
   <si>
@@ -204,100 +159,10 @@
     <t>Kocherga</t>
   </si>
   <si>
-    <t>Kyrylivna</t>
-  </si>
-  <si>
     <t>kocherga@email.com</t>
   </si>
   <si>
     <t>kocherga</t>
-  </si>
-  <si>
-    <t>Sihav</t>
-  </si>
-  <si>
-    <t>Indiya</t>
-  </si>
-  <si>
-    <t>Shuvar</t>
-  </si>
-  <si>
-    <t>Santa Monika</t>
-  </si>
-  <si>
-    <t>Pidzamche</t>
-  </si>
-  <si>
-    <t>Centry</t>
-  </si>
-  <si>
-    <t>Himichna</t>
-  </si>
-  <si>
-    <t>Shota</t>
-  </si>
-  <si>
-    <t>Zelena</t>
-  </si>
-  <si>
-    <t>Kryva</t>
-  </si>
-  <si>
-    <t>Gorihova</t>
-  </si>
-  <si>
-    <t>Kalyuzhna</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>79001</t>
-  </si>
-  <si>
-    <t>79002</t>
-  </si>
-  <si>
-    <t>79003</t>
-  </si>
-  <si>
-    <t>79004</t>
-  </si>
-  <si>
-    <t>79005</t>
-  </si>
-  <si>
-    <t>79006</t>
   </si>
 </sst>
 </file>
@@ -687,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,59 +643,35 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="F2" s="4">
         <v>111111</v>
       </c>
       <c r="G2" s="4">
         <v>111111</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="5">
-        <v>111111</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="5">
-        <v>673660001</v>
-      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="5"/>
       <c r="S2" s="2" t="s">
         <v>4</v>
       </c>
@@ -838,19 +679,17 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>36</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C3" s="4"/>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F3" s="4">
         <v>111111</v>
@@ -858,39 +697,17 @@
       <c r="G3" s="4">
         <v>111111</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="5">
-        <v>222222</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="5">
-        <v>673660002</v>
-      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="5"/>
       <c r="S3" s="2" t="s">
         <v>4</v>
       </c>
@@ -898,59 +715,35 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="F4" s="4">
         <v>111111</v>
       </c>
       <c r="G4" s="4">
         <v>111111</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="5">
-        <v>333333</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="5">
-        <v>673660003</v>
-      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="5"/>
       <c r="S4" s="2" t="s">
         <v>4</v>
       </c>
@@ -958,19 +751,17 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C5" s="4"/>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F5" s="4">
         <v>111111</v>
@@ -978,39 +769,17 @@
       <c r="G5" s="4">
         <v>111111</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" s="5">
-        <v>444444</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5" s="5">
-        <v>673660004</v>
-      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="5"/>
       <c r="S5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1018,19 +787,17 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C6" s="4"/>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F6" s="4">
         <v>111111</v>
@@ -1038,39 +805,17 @@
       <c r="G6" s="4">
         <v>111111</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" s="5">
-        <v>555555</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R6" s="5">
-        <v>673660005</v>
-      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="5"/>
       <c r="S6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1078,19 +823,17 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C7" s="4"/>
       <c r="D7" s="6" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F7" s="4">
         <v>111111</v>
@@ -1098,39 +841,17 @@
       <c r="G7" s="4">
         <v>111111</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P7" s="5">
-        <v>666666</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R7" s="5">
-        <v>673660006</v>
-      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="5"/>
       <c r="S7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1138,19 +859,17 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>61</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="6" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F8" s="4">
         <v>111111</v>
@@ -1158,39 +877,17 @@
       <c r="G8" s="4">
         <v>111111</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" s="5">
-        <v>777777</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R8" s="5">
-        <v>673660007</v>
-      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="5"/>
       <c r="S8" s="2" t="s">
         <v>4</v>
       </c>

</xml_diff>